<commit_message>
add opt raw table and change the compare voltage to Vref
</commit_message>
<xml_diff>
--- a/ra_exploer/examples/Seal WVTR_TR2_All.xlsx
+++ b/ra_exploer/examples/Seal WVTR_TR2_All.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dimsp\Documents\Projects\td_toolkits_reconstruc\ra_exploer\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\td_toolkits_reconstruc\ra_exploer\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5405EDE5-552F-44E7-9A7E-50D7A3AB3840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22815" yWindow="6600" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23745" yWindow="6600" windowWidth="20910" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Seal_WVTR" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Seal_WVTR!$A$1:$I$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Seal_WVTR!$A$1:$J$14</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
   <si>
     <t>Y軸項目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,14 +45,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Measure condition-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Measure condition-2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Y軸數值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -70,14 +61,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>80℃ / 90% RH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>膜厚 300um</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>協立</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -93,15 +76,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>膜厚 300um</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>WVTR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>80℃ / 90% RH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -156,14 +131,26 @@
   </si>
   <si>
     <t>N.A.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>溫度(°C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>濕度(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>膜厚(um)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,12 +178,6 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="微軟正黑體"/>
-      <family val="2"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="10"/>
@@ -247,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,13 +242,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -291,13 +266,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>187698</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>52668</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>490257</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>161365</xdr:rowOff>
@@ -307,7 +282,7 @@
         <xdr:cNvPr id="2" name="文字方塊 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -378,13 +353,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>168648</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>81243</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>471207</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>21851</xdr:rowOff>
@@ -394,7 +369,7 @@
         <xdr:cNvPr id="3" name="文字方塊 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -465,13 +440,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>195542</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>25214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>498101</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>155203</xdr:rowOff>
@@ -481,7 +456,7 @@
         <xdr:cNvPr id="5" name="文字方塊 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -815,14 +790,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -832,13 +807,13 @@
     <col min="3" max="3" width="7.625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.25" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="23.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="77.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="3"/>
+    <col min="6" max="8" width="12" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="77.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -852,396 +827,438 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <v>69.2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1">
+        <v>80</v>
+      </c>
+      <c r="G2" s="1">
+        <v>90</v>
+      </c>
+      <c r="H2" s="1">
+        <v>300</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="1">
         <v>87.1</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1">
+        <v>80</v>
+      </c>
+      <c r="G3" s="1">
+        <v>90</v>
+      </c>
+      <c r="H3" s="1">
+        <v>300</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5">
+        <v>197</v>
+      </c>
+      <c r="F4" s="1">
+        <v>80</v>
+      </c>
+      <c r="G4" s="1">
+        <v>90</v>
+      </c>
+      <c r="H4" s="1">
+        <v>300</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5">
+        <v>250</v>
+      </c>
+      <c r="F5" s="1">
+        <v>80</v>
+      </c>
+      <c r="G5" s="1">
+        <v>90</v>
+      </c>
+      <c r="H5" s="1">
+        <v>300</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="E6" s="5">
+        <v>177</v>
+      </c>
+      <c r="F6" s="1">
+        <v>80</v>
+      </c>
+      <c r="G6" s="1">
+        <v>90</v>
+      </c>
+      <c r="H6" s="1">
+        <v>300</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="6">
-        <v>197</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="J6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="6">
-        <v>250</v>
-      </c>
-      <c r="F5" s="7" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="5">
+        <v>281</v>
+      </c>
+      <c r="F7" s="1">
+        <v>80</v>
+      </c>
+      <c r="G7" s="1">
+        <v>90</v>
+      </c>
+      <c r="H7" s="1">
+        <v>300</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6">
-        <v>177</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="6">
-        <v>281</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1">
         <v>101</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>27</v>
+      <c r="F8" s="1">
+        <v>80</v>
+      </c>
+      <c r="G8" s="1">
+        <v>90</v>
+      </c>
+      <c r="H8" s="1">
+        <v>300</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1">
         <v>98</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>27</v>
+      <c r="F9" s="1">
+        <v>80</v>
+      </c>
+      <c r="G9" s="1">
+        <v>90</v>
+      </c>
+      <c r="H9" s="1">
+        <v>300</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1">
         <v>72</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>27</v>
+      <c r="F10" s="1">
+        <v>80</v>
+      </c>
+      <c r="G10" s="1">
+        <v>90</v>
+      </c>
+      <c r="H10" s="1">
+        <v>300</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1">
+        <v>80</v>
+      </c>
+      <c r="G11" s="1">
+        <v>90</v>
+      </c>
+      <c r="H11" s="1">
+        <v>300</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="5">
-        <v>56</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E12" s="1">
         <v>101</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>27</v>
+      <c r="F12" s="1">
+        <v>80</v>
+      </c>
+      <c r="G12" s="1">
+        <v>90</v>
+      </c>
+      <c r="H12" s="1">
+        <v>300</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1">
         <v>72</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>27</v>
+      <c r="F13" s="1">
+        <v>80</v>
+      </c>
+      <c r="G13" s="1">
+        <v>90</v>
+      </c>
+      <c r="H13" s="1">
+        <v>300</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="5">
+        <v>22</v>
+      </c>
+      <c r="E14" s="4">
         <v>60</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>27</v>
+      <c r="F14" s="1">
+        <v>80</v>
+      </c>
+      <c r="G14" s="1">
+        <v>90</v>
+      </c>
+      <c r="H14" s="1">
+        <v>300</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>